<commit_message>
#update 02.21 - construção painel 1
</commit_message>
<xml_diff>
--- a/data/CVM/Dados_CVM/TratamentoManual/cia_construcao.xlsx
+++ b/data/CVM/Dados_CVM/TratamentoManual/cia_construcao.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Convidado\ownCloud\Documentos\RAYMUNDO\Analises\Relatorio\Dados_CVM\TratamentoManual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raymundo\Documentos\R\painel-indicadores\data\CVM\Dados_CVM\TratamentoManual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1634B575-5C0B-480E-AE13-D915DE7E76D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3337D37-D8CD-4932-B988-1FF71EB6764D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C2D8E81A-D474-4C7F-B3F1-CFF3898DBD13}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C2D8E81A-D474-4C7F-B3F1-CFF3898DBD13}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1031,9 +1031,6 @@
     <t>EZ Inc</t>
   </si>
   <si>
-    <t>Ez Tec</t>
-  </si>
-  <si>
     <t>HBR Realty</t>
   </si>
   <si>
@@ -1094,14 +1091,25 @@
     <t>41.10-7-00 - Incorporação de empreendimentos imobiliários
 68.10-2-01 - Compra e venda de imóveis próprios
 68.10-2-02 - Aluguel de imóveis próprios</t>
+  </si>
+  <si>
+    <t>EZ Tec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1129,12 +1137,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1461,23 +1472,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABACBB8E-E414-4A68-98E8-4867E4F2B669}">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.81640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="66" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7109375" style="2"/>
+    <col min="8" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1500,7 +1511,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>25275</v>
       </c>
@@ -1523,7 +1534,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>11975</v>
       </c>
@@ -1546,7 +1557,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>4723</v>
       </c>
@@ -1569,18 +1580,18 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>27340</v>
       </c>
       <c r="B5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="C5" t="s">
-        <v>271</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>66</v>
@@ -1589,10 +1600,10 @@
         <v>78</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>13030</v>
       </c>
@@ -1600,7 +1611,7 @@
         <v>109</v>
       </c>
       <c r="C6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>229</v>
@@ -1612,7 +1623,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>21148</v>
       </c>
@@ -1635,7 +1646,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>4863</v>
       </c>
@@ -1655,7 +1666,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>25100</v>
       </c>
@@ -1678,7 +1689,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>14460</v>
       </c>
@@ -1686,7 +1697,7 @@
         <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>231</v>
@@ -1701,7 +1712,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>21091</v>
       </c>
@@ -1724,7 +1735,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="174" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>21350</v>
       </c>
@@ -1747,7 +1758,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>25909</v>
       </c>
@@ -1758,7 +1769,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>66</v>
@@ -1770,7 +1781,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="174" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>5762</v>
       </c>
@@ -1793,7 +1804,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>5770</v>
       </c>
@@ -1816,7 +1827,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>20524</v>
       </c>
@@ -1839,7 +1850,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>25380</v>
       </c>
@@ -1862,7 +1873,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>20770</v>
       </c>
@@ -1873,7 +1884,7 @@
         <v>18</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>66</v>
@@ -1885,7 +1896,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>20630</v>
       </c>
@@ -1895,7 +1906,7 @@
       <c r="C19" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>238</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -1905,7 +1916,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>26336</v>
       </c>
@@ -1928,7 +1939,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>16101</v>
       </c>
@@ -1951,7 +1962,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>26115</v>
       </c>
@@ -1962,7 +1973,7 @@
         <v>21</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>68</v>
@@ -1974,7 +1985,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>25402</v>
       </c>
@@ -1985,7 +1996,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>67</v>
@@ -1997,7 +2008,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>20877</v>
       </c>
@@ -2020,7 +2031,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24279</v>
       </c>
@@ -2043,7 +2054,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="360" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25992</v>
       </c>
@@ -2054,7 +2065,7 @@
         <v>25</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>65</v>
@@ -2066,7 +2077,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>20605</v>
       </c>
@@ -2089,7 +2100,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>7811</v>
       </c>
@@ -2112,7 +2123,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>25798</v>
       </c>
@@ -2123,7 +2134,7 @@
         <v>28</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>66</v>
@@ -2135,7 +2146,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>25062</v>
       </c>
@@ -2158,7 +2169,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>23272</v>
       </c>
@@ -2166,7 +2177,7 @@
         <v>134</v>
       </c>
       <c r="C31" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>248</v>
@@ -2181,7 +2192,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>20370</v>
       </c>
@@ -2204,7 +2215,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>25119</v>
       </c>
@@ -2227,7 +2238,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>4782</v>
       </c>
@@ -2247,7 +2258,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>24902</v>
       </c>
@@ -2270,7 +2281,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>21067</v>
       </c>
@@ -2293,7 +2304,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>20915</v>
       </c>
@@ -2316,7 +2327,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>20982</v>
       </c>
@@ -2324,7 +2335,7 @@
         <v>141</v>
       </c>
       <c r="C38" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>242</v>
@@ -2339,7 +2350,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>21180</v>
       </c>
@@ -2359,7 +2370,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>25143</v>
       </c>
@@ -2382,7 +2393,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>25305</v>
       </c>
@@ -2405,7 +2416,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="232" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>13773</v>
       </c>
@@ -2428,7 +2439,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>20478</v>
       </c>
@@ -2436,7 +2447,7 @@
         <v>146</v>
       </c>
       <c r="C43" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>235</v>
@@ -2451,7 +2462,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>25070</v>
       </c>
@@ -2474,7 +2485,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>9717</v>
       </c>
@@ -2494,7 +2505,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="315" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>24236</v>
       </c>
@@ -2517,7 +2528,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>20451</v>
       </c>
@@ -2540,7 +2551,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>16306</v>
       </c>
@@ -2563,7 +2574,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>23540</v>
       </c>
@@ -2580,7 +2591,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>10880</v>
       </c>
@@ -2603,7 +2614,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>23957</v>
       </c>
@@ -2623,7 +2634,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>21040</v>
       </c>
@@ -2643,7 +2654,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>20435</v>
       </c>
@@ -2666,7 +2677,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>11207</v>
       </c>
@@ -2674,7 +2685,7 @@
         <v>156</v>
       </c>
       <c r="C54" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>215</v>
@@ -2686,7 +2697,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>25844</v>
       </c>
@@ -2697,7 +2708,7 @@
         <v>53</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>66</v>
@@ -2709,7 +2720,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>26255</v>
       </c>
@@ -2732,7 +2743,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>21130</v>
       </c>
@@ -2755,7 +2766,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>22780</v>
       </c>
@@ -2775,7 +2786,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="116" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>25437</v>
       </c>
@@ -2786,7 +2797,7 @@
         <v>57</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>71</v>
@@ -2798,7 +2809,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>20702</v>
       </c>
@@ -2821,7 +2832,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>27189</v>
       </c>
@@ -2832,7 +2843,7 @@
         <v>59</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>65</v>
@@ -2844,7 +2855,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>23604</v>
       </c>
@@ -2852,7 +2863,7 @@
         <v>164</v>
       </c>
       <c r="C62" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>250</v>
@@ -2867,7 +2878,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>25976</v>
       </c>
@@ -2878,7 +2889,7 @@
         <v>61</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>66</v>
@@ -2890,181 +2901,181 @@
         <v>203</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C64"/>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C65"/>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C66"/>
     </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C67"/>
     </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C68"/>
     </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C69"/>
     </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C70"/>
     </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C71"/>
     </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C72"/>
     </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C73"/>
     </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C74"/>
     </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C75"/>
     </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C76"/>
     </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C77"/>
     </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C78"/>
     </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C79"/>
     </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C80"/>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C81"/>
     </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C82"/>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C83"/>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C84"/>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C85"/>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C86"/>
     </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C87"/>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C88"/>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C89"/>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C90"/>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C91"/>
     </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C92"/>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C93"/>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C94"/>
     </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C95"/>
     </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C96"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C97"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C98"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C99"/>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C100"/>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C101"/>
     </row>
-    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C102"/>
     </row>
-    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C103"/>
     </row>
-    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C104"/>
     </row>
-    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C105"/>
     </row>
-    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C106"/>
     </row>
-    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C107"/>
     </row>
-    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C108"/>
     </row>
-    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C109"/>
     </row>
-    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C110"/>
     </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C111"/>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C112"/>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C113"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C114"/>
     </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C115"/>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C116"/>
     </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C117"/>
     </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C118"/>
     </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C119"/>
     </row>
-    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C120"/>
     </row>
-    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C121"/>
     </row>
-    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C122"/>
     </row>
   </sheetData>
@@ -3086,14 +3097,14 @@
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3104,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>25275</v>
       </c>
@@ -3115,7 +3126,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>11975</v>
       </c>
@@ -3126,7 +3137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13030</v>
       </c>
@@ -3137,7 +3148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4723</v>
       </c>
@@ -3148,7 +3159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>21148</v>
       </c>
@@ -3159,7 +3170,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4863</v>
       </c>
@@ -3170,7 +3181,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>20630</v>
       </c>
@@ -3181,7 +3192,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>25100</v>
       </c>
@@ -3192,7 +3203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>14460</v>
       </c>
@@ -3203,7 +3214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>21091</v>
       </c>
@@ -3214,7 +3225,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>21350</v>
       </c>
@@ -3225,7 +3236,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>25909</v>
       </c>
@@ -3236,7 +3247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5762</v>
       </c>
@@ -3247,7 +3258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5770</v>
       </c>
@@ -3258,7 +3269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>20524</v>
       </c>
@@ -3269,7 +3280,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>25380</v>
       </c>
@@ -3280,7 +3291,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>20770</v>
       </c>
@@ -3291,7 +3302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>26336</v>
       </c>
@@ -3302,7 +3313,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>16101</v>
       </c>
@@ -3313,7 +3324,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>26115</v>
       </c>
@@ -3324,7 +3335,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>25402</v>
       </c>
@@ -3335,7 +3346,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>20877</v>
       </c>
@@ -3346,7 +3357,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>24279</v>
       </c>
@@ -3357,7 +3368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>25992</v>
       </c>
@@ -3368,7 +3379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>20605</v>
       </c>
@@ -3379,7 +3390,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>7811</v>
       </c>
@@ -3390,7 +3401,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>25798</v>
       </c>
@@ -3401,7 +3412,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>25062</v>
       </c>
@@ -3412,7 +3423,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>23272</v>
       </c>
@@ -3423,7 +3434,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>20370</v>
       </c>
@@ -3434,7 +3445,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>25119</v>
       </c>
@@ -3445,7 +3456,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>4782</v>
       </c>
@@ -3456,7 +3467,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>24902</v>
       </c>
@@ -3467,7 +3478,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>21067</v>
       </c>
@@ -3478,7 +3489,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>20915</v>
       </c>
@@ -3489,7 +3500,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>20982</v>
       </c>
@@ -3500,7 +3511,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>21180</v>
       </c>
@@ -3511,7 +3522,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>25143</v>
       </c>
@@ -3522,7 +3533,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>25305</v>
       </c>
@@ -3533,7 +3544,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>13773</v>
       </c>
@@ -3544,7 +3555,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>20478</v>
       </c>
@@ -3555,7 +3566,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>25070</v>
       </c>
@@ -3566,7 +3577,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>9717</v>
       </c>
@@ -3577,7 +3588,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>24236</v>
       </c>
@@ -3588,7 +3599,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>20451</v>
       </c>
@@ -3599,7 +3610,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>16306</v>
       </c>
@@ -3610,7 +3621,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>10880</v>
       </c>
@@ -3621,7 +3632,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>23957</v>
       </c>
@@ -3632,7 +3643,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>21040</v>
       </c>
@@ -3643,7 +3654,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>20435</v>
       </c>
@@ -3654,7 +3665,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>11207</v>
       </c>
@@ -3665,7 +3676,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>25844</v>
       </c>
@@ -3676,7 +3687,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>26255</v>
       </c>
@@ -3687,7 +3698,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>21130</v>
       </c>
@@ -3698,7 +3709,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>22780</v>
       </c>
@@ -3709,7 +3720,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>25437</v>
       </c>
@@ -3720,7 +3731,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>20702</v>
       </c>
@@ -3731,7 +3742,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>27189</v>
       </c>
@@ -3742,7 +3753,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>23604</v>
       </c>
@@ -3753,7 +3764,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>25976</v>
       </c>

</xml_diff>